<commit_message>
added test print statements to stage 004 for SH testing
</commit_message>
<xml_diff>
--- a/raw_data/user_and_data_parameters/user_and_data_params.xlsx
+++ b/raw_data/user_and_data_parameters/user_and_data_params.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Matthew_Eves\Documents\HSMA_local\Greener NHS funded development\01. Final files\raw_data\user_and_data_parameters\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Matthew_Eves\Documents\HSMA_local\Greener NHS funded development\shine\raw_data\user_and_data_parameters\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDE05BB0-9F6C-486D-9D48-5921BFD2899D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD252D3C-02D0-4337-BB9F-F4A13B527A3D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2295" yWindow="2295" windowWidth="38700" windowHeight="15345" tabRatio="722" xr2:uid="{24475980-04B6-4043-8A41-34925FD08545}"/>
+    <workbookView xWindow="1875" yWindow="1575" windowWidth="38700" windowHeight="15105" tabRatio="722" firstSheet="2" activeTab="3" xr2:uid="{24475980-04B6-4043-8A41-34925FD08545}"/>
   </bookViews>
   <sheets>
     <sheet name="AssignFieldNamesToVars" sheetId="1" r:id="rId1"/>
@@ -104,7 +104,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="643" uniqueCount="559">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="627" uniqueCount="544">
   <si>
     <t>field_name_in_service_data</t>
   </si>
@@ -2416,60 +2416,6 @@
     <t>A text label to indicate the appointment type, e.g. face to face, telephone, etc.</t>
   </si>
   <si>
-    <t>Not Known</t>
-  </si>
-  <si>
-    <t>White - British</t>
-  </si>
-  <si>
-    <t>Black or Black British - Caribbean</t>
-  </si>
-  <si>
-    <t>White - Other</t>
-  </si>
-  <si>
-    <t>Black or Black British - Other</t>
-  </si>
-  <si>
-    <t>Asian or Asian British - Pakistani</t>
-  </si>
-  <si>
-    <t>Asian or Asian British - Bangladeshi</t>
-  </si>
-  <si>
-    <t>Other Ethnic Groups - Other</t>
-  </si>
-  <si>
-    <t>Mixed - Other</t>
-  </si>
-  <si>
-    <t>Mixed - White and Black Caribbean</t>
-  </si>
-  <si>
-    <t>Asian or Asian British - Indian</t>
-  </si>
-  <si>
-    <t>Not stated</t>
-  </si>
-  <si>
-    <t>Black or Black British - African</t>
-  </si>
-  <si>
-    <t>Asian or Asian British - Other</t>
-  </si>
-  <si>
-    <t>White - Irish</t>
-  </si>
-  <si>
-    <t>Other Ethnic Groups - Chinese</t>
-  </si>
-  <si>
-    <t>Mixed - White and Asian</t>
-  </si>
-  <si>
-    <t>Mixed - White and Black African</t>
-  </si>
-  <si>
     <t>nhs_orange - #ED8B00</t>
   </si>
   <si>
@@ -2680,6 +2626,15 @@
   </si>
   <si>
     <t xml:space="preserve">The value entered represents the size of the samples when running multiple iterations of the machine learning models. This may require some experimentation due to the random nature of selecting the samples (if a sample is randomly selected containing only patients who dna or only attend, the model will crash, because it must have TWO statuses present). For context, in testing, on a data set with c.40k records, a sample size of 250 was used successfully. </t>
+  </si>
+  <si>
+    <t>GUM</t>
+  </si>
+  <si>
+    <t>Contraception</t>
+  </si>
+  <si>
+    <t>Test Service</t>
   </si>
 </sst>
 </file>
@@ -3895,9 +3850,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FC5F284D-2005-4845-81EE-CD68A6EE6E51}">
   <dimension ref="A1:E20"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B17" sqref="B17"/>
+      <selection pane="bottomLeft" activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4398,7 +4353,7 @@
         <v>329</v>
       </c>
       <c r="J2" s="40" t="s">
-        <v>509</v>
+        <v>491</v>
       </c>
     </row>
     <row r="3" spans="1:17" ht="45" x14ac:dyDescent="0.25">
@@ -4406,22 +4361,22 @@
         <v>322</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>502</v>
+        <v>484</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>503</v>
+        <v>485</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>504</v>
+        <v>486</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>505</v>
+        <v>487</v>
       </c>
       <c r="F3" s="8" t="s">
-        <v>506</v>
+        <v>488</v>
       </c>
       <c r="G3" s="8" t="s">
-        <v>507</v>
+        <v>489</v>
       </c>
       <c r="H3" s="39" t="s">
         <v>330</v>
@@ -4430,22 +4385,22 @@
         <v>322</v>
       </c>
       <c r="K3" s="8" t="s">
-        <v>502</v>
+        <v>484</v>
       </c>
       <c r="L3" s="8" t="s">
-        <v>503</v>
+        <v>485</v>
       </c>
       <c r="M3" s="8" t="s">
-        <v>504</v>
+        <v>486</v>
       </c>
       <c r="N3" s="8" t="s">
-        <v>505</v>
+        <v>487</v>
       </c>
       <c r="O3" s="8" t="s">
-        <v>506</v>
+        <v>488</v>
       </c>
       <c r="P3" s="8" t="s">
-        <v>507</v>
+        <v>489</v>
       </c>
       <c r="Q3" s="39" t="s">
         <v>330</v>
@@ -4477,7 +4432,7 @@
         <v>0</v>
       </c>
       <c r="J4" s="50" t="s">
-        <v>501</v>
+        <v>483</v>
       </c>
       <c r="K4" s="49">
         <v>1.2E-2</v>
@@ -4526,7 +4481,7 @@
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6" s="52" t="s">
-        <v>508</v>
+        <v>490</v>
       </c>
       <c r="B6" s="59">
         <v>0.77799999999999991</v>
@@ -6507,37 +6462,37 @@
     </row>
     <row r="365" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A365" s="1" t="s">
-        <v>515</v>
+        <v>497</v>
       </c>
     </row>
     <row r="366" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A366" t="s">
-        <v>516</v>
+        <v>498</v>
       </c>
     </row>
     <row r="367" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A367" t="s">
-        <v>517</v>
+        <v>499</v>
       </c>
     </row>
     <row r="368" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A368" t="s">
-        <v>514</v>
+        <v>496</v>
       </c>
     </row>
     <row r="371" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A371" t="s">
-        <v>541</v>
+        <v>523</v>
       </c>
     </row>
     <row r="372" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A372" t="s">
-        <v>542</v>
+        <v>524</v>
       </c>
     </row>
     <row r="373" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A373" t="s">
-        <v>543</v>
+        <v>525</v>
       </c>
     </row>
   </sheetData>
@@ -6635,7 +6590,7 @@
         <v>303</v>
       </c>
       <c r="C5" s="31" t="s">
-        <v>496</v>
+        <v>478</v>
       </c>
       <c r="D5" s="9" t="str">
         <f>VLOOKUP(C5,reference_lists!A236:B243,2,FALSE)</f>
@@ -6942,7 +6897,7 @@
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6982,13 +6937,13 @@
     </row>
     <row r="3" spans="1:4" ht="120" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>557</v>
+        <v>539</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>558</v>
+        <v>540</v>
       </c>
       <c r="C3" s="7">
-        <v>250</v>
+        <v>100</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>49</v>
@@ -7004,11 +6959,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{02862E97-ED6B-45A0-9477-766967619C86}">
   <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C5" sqref="C5"/>
+      <selection pane="bottomRight" activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7071,7 +7026,9 @@
       <c r="B4" s="21" t="s">
         <v>256</v>
       </c>
-      <c r="C4" s="3"/>
+      <c r="C4" s="3" t="s">
+        <v>211</v>
+      </c>
       <c r="D4" s="4" t="s">
         <v>259</v>
       </c>
@@ -7083,7 +7040,9 @@
       <c r="B5" s="21" t="s">
         <v>457</v>
       </c>
-      <c r="C5" s="3"/>
+      <c r="C5" s="3" t="s">
+        <v>543</v>
+      </c>
       <c r="D5" s="4" t="s">
         <v>258</v>
       </c>
@@ -7111,7 +7070,7 @@
   <dimension ref="A2:J26"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="K8" sqref="K8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7147,7 +7106,9 @@
       <c r="C3" s="21" t="s">
         <v>344</v>
       </c>
-      <c r="D3" s="3"/>
+      <c r="D3" s="3">
+        <v>2</v>
+      </c>
       <c r="E3" s="21" t="s">
         <v>49</v>
       </c>
@@ -7175,39 +7136,71 @@
         <v>339</v>
       </c>
       <c r="I6" s="44" t="s">
-        <v>556</v>
+        <v>538</v>
       </c>
       <c r="J6" s="44" t="s">
-        <v>555</v>
+        <v>537</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>1</v>
       </c>
-      <c r="B7" s="43"/>
-      <c r="C7" s="43"/>
-      <c r="D7" s="47"/>
-      <c r="E7" s="47"/>
-      <c r="F7" s="47"/>
-      <c r="G7" s="47"/>
-      <c r="H7" s="43"/>
-      <c r="I7" s="57"/>
-      <c r="J7" s="43"/>
+      <c r="B7" s="43" t="s">
+        <v>541</v>
+      </c>
+      <c r="C7" s="43" t="s">
+        <v>334</v>
+      </c>
+      <c r="D7" s="47">
+        <v>10</v>
+      </c>
+      <c r="E7" s="47">
+        <v>20</v>
+      </c>
+      <c r="F7" s="47">
+        <v>16</v>
+      </c>
+      <c r="G7" s="47">
+        <v>45</v>
+      </c>
+      <c r="H7" s="43" t="s">
+        <v>341</v>
+      </c>
+      <c r="I7" s="57">
+        <v>0.5</v>
+      </c>
+      <c r="J7" s="43">
+        <v>1</v>
+      </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>2</v>
       </c>
-      <c r="B8" s="43"/>
-      <c r="C8" s="43"/>
+      <c r="B8" s="43" t="s">
+        <v>542</v>
+      </c>
+      <c r="C8" s="43" t="s">
+        <v>335</v>
+      </c>
       <c r="D8" s="47"/>
       <c r="E8" s="47"/>
-      <c r="F8" s="47"/>
-      <c r="G8" s="47"/>
-      <c r="H8" s="43"/>
-      <c r="I8" s="57"/>
-      <c r="J8" s="43"/>
+      <c r="F8" s="47">
+        <v>16</v>
+      </c>
+      <c r="G8" s="47">
+        <v>49</v>
+      </c>
+      <c r="H8" s="43" t="s">
+        <v>343</v>
+      </c>
+      <c r="I8" s="57">
+        <v>0.5</v>
+      </c>
+      <c r="J8" s="43">
+        <v>1</v>
+      </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9">
@@ -7864,7 +7857,7 @@
   <dimension ref="A1:B20"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7892,15 +7885,15 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="13" t="s">
-        <v>484</v>
+        <v>53</v>
       </c>
       <c r="B3" s="14" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="13" t="s">
-        <v>488</v>
+        <v>52</v>
       </c>
       <c r="B4" s="14" t="s">
         <v>52</v>
@@ -7908,123 +7901,75 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="13" t="s">
-        <v>491</v>
+        <v>51</v>
       </c>
       <c r="B5" s="14" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="13" t="s">
-        <v>483</v>
+        <v>54</v>
       </c>
       <c r="B6" s="14" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="13" t="s">
-        <v>490</v>
+        <v>56</v>
       </c>
       <c r="B7" s="14" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" s="13" t="s">
-        <v>480</v>
-      </c>
-      <c r="B8" s="14" t="s">
-        <v>53</v>
-      </c>
+      <c r="A8" s="13"/>
+      <c r="B8" s="14"/>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" s="3" t="s">
-        <v>482</v>
-      </c>
-      <c r="B9" s="14" t="s">
-        <v>53</v>
-      </c>
+      <c r="A9" s="3"/>
+      <c r="B9" s="14"/>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" s="3" t="s">
-        <v>486</v>
-      </c>
-      <c r="B10" s="14" t="s">
-        <v>51</v>
-      </c>
+      <c r="A10" s="3"/>
+      <c r="B10" s="14"/>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" s="3" t="s">
-        <v>494</v>
-      </c>
-      <c r="B11" s="14" t="s">
-        <v>51</v>
-      </c>
+      <c r="A11" s="3"/>
+      <c r="B11" s="14"/>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" s="3" t="s">
-        <v>495</v>
-      </c>
-      <c r="B12" s="14" t="s">
-        <v>51</v>
-      </c>
+      <c r="A12" s="3"/>
+      <c r="B12" s="14"/>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" s="3" t="s">
-        <v>487</v>
-      </c>
-      <c r="B13" s="14" t="s">
-        <v>51</v>
-      </c>
+      <c r="A13" s="3"/>
+      <c r="B13" s="14"/>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" s="3" t="s">
-        <v>489</v>
-      </c>
-      <c r="B14" s="14" t="s">
-        <v>54</v>
-      </c>
+      <c r="A14" s="3"/>
+      <c r="B14" s="14"/>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" s="3" t="s">
-        <v>493</v>
-      </c>
-      <c r="B15" s="14" t="s">
-        <v>54</v>
-      </c>
+      <c r="A15" s="3"/>
+      <c r="B15" s="14"/>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16" s="3" t="s">
-        <v>485</v>
-      </c>
-      <c r="B16" s="14" t="s">
-        <v>54</v>
-      </c>
+      <c r="A16" s="3"/>
+      <c r="B16" s="14"/>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" s="3" t="s">
-        <v>479</v>
-      </c>
-      <c r="B17" s="14" t="s">
-        <v>56</v>
-      </c>
+      <c r="A17" s="3"/>
+      <c r="B17" s="14"/>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" s="3" t="s">
-        <v>492</v>
-      </c>
-      <c r="B18" s="14" t="s">
-        <v>56</v>
-      </c>
+      <c r="A18" s="3"/>
+      <c r="B18" s="14"/>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" s="3" t="s">
-        <v>481</v>
-      </c>
-      <c r="B19" s="14" t="s">
-        <v>56</v>
-      </c>
+      <c r="A19" s="3"/>
+      <c r="B19" s="14"/>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="3"/>
@@ -8055,7 +8000,7 @@
   <dimension ref="A1:F18"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8098,7 +8043,7 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="13" t="s">
-        <v>478</v>
+        <v>54</v>
       </c>
       <c r="B5" s="14" t="s">
         <v>78</v>
@@ -8336,10 +8281,10 @@
         <v>320</v>
       </c>
       <c r="D1" s="35" t="s">
-        <v>498</v>
+        <v>480</v>
       </c>
       <c r="E1" s="35" t="s">
-        <v>499</v>
+        <v>481</v>
       </c>
       <c r="F1" s="36" t="s">
         <v>321</v>
@@ -8356,10 +8301,10 @@
         <v>317</v>
       </c>
       <c r="D2" s="34" t="s">
-        <v>497</v>
+        <v>479</v>
       </c>
       <c r="E2" s="34" t="s">
-        <v>500</v>
+        <v>482</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -8434,7 +8379,7 @@
     </row>
     <row r="16" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A16" s="28" t="s">
-        <v>510</v>
+        <v>492</v>
       </c>
       <c r="B16" s="53"/>
       <c r="C16" s="53"/>
@@ -8443,7 +8388,7 @@
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>526</v>
+        <v>508</v>
       </c>
       <c r="B17" s="2"/>
       <c r="C17" s="2"/>
@@ -8452,7 +8397,7 @@
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>511</v>
+        <v>493</v>
       </c>
       <c r="B18" s="2"/>
       <c r="C18" s="2"/>
@@ -8461,7 +8406,7 @@
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
-        <v>512</v>
+        <v>494</v>
       </c>
       <c r="B19" s="2"/>
       <c r="C19" s="2"/>
@@ -8470,7 +8415,7 @@
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
-        <v>513</v>
+        <v>495</v>
       </c>
       <c r="B20" s="2"/>
       <c r="C20" s="2"/>
@@ -8479,12 +8424,12 @@
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
-        <v>517</v>
+        <v>499</v>
       </c>
     </row>
     <row r="24" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A24" s="28" t="s">
-        <v>521</v>
+        <v>503</v>
       </c>
       <c r="B24" s="53"/>
       <c r="C24" s="53"/>
@@ -8493,7 +8438,7 @@
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
-        <v>518</v>
+        <v>500</v>
       </c>
       <c r="B25" s="2"/>
       <c r="C25" s="2"/>
@@ -8502,7 +8447,7 @@
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
-        <v>519</v>
+        <v>501</v>
       </c>
       <c r="B26" s="2"/>
       <c r="C26" s="2"/>
@@ -8511,7 +8456,7 @@
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
-        <v>520</v>
+        <v>502</v>
       </c>
       <c r="B27" s="2"/>
       <c r="C27" s="2"/>
@@ -8520,16 +8465,16 @@
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="54" t="s">
-        <v>522</v>
+        <v>504</v>
       </c>
       <c r="B28" s="54" t="s">
-        <v>523</v>
+        <v>505</v>
       </c>
       <c r="C28" s="54" t="s">
-        <v>524</v>
+        <v>506</v>
       </c>
       <c r="D28" s="54" t="s">
-        <v>525</v>
+        <v>507</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
@@ -8548,7 +8493,7 @@
     </row>
     <row r="32" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A32" s="28" t="s">
-        <v>527</v>
+        <v>509</v>
       </c>
       <c r="B32" s="53"/>
       <c r="C32" s="53"/>
@@ -8557,7 +8502,7 @@
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
-        <v>528</v>
+        <v>510</v>
       </c>
       <c r="B33" s="2"/>
       <c r="C33" s="2"/>
@@ -8566,7 +8511,7 @@
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
-        <v>529</v>
+        <v>511</v>
       </c>
       <c r="B34" s="2"/>
       <c r="C34" s="2"/>
@@ -8575,7 +8520,7 @@
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
-        <v>530</v>
+        <v>512</v>
       </c>
       <c r="B35" s="2"/>
       <c r="C35" s="2"/>
@@ -8584,7 +8529,7 @@
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
-        <v>531</v>
+        <v>513</v>
       </c>
       <c r="B36" s="2"/>
       <c r="C36" s="2"/>
@@ -8593,7 +8538,7 @@
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
-        <v>532</v>
+        <v>514</v>
       </c>
       <c r="B37" s="2"/>
       <c r="C37" s="2"/>
@@ -8602,7 +8547,7 @@
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
-        <v>533</v>
+        <v>515</v>
       </c>
       <c r="B38" s="2"/>
       <c r="C38" s="2"/>
@@ -8611,7 +8556,7 @@
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
-        <v>534</v>
+        <v>516</v>
       </c>
       <c r="B39" s="2"/>
       <c r="C39" s="2"/>
@@ -8620,7 +8565,7 @@
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
-        <v>535</v>
+        <v>517</v>
       </c>
       <c r="B40" s="2"/>
       <c r="C40" s="2"/>
@@ -8629,7 +8574,7 @@
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" s="2" t="s">
-        <v>536</v>
+        <v>518</v>
       </c>
       <c r="B41" s="2"/>
       <c r="C41" s="2"/>
@@ -8638,7 +8583,7 @@
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" s="2" t="s">
-        <v>539</v>
+        <v>521</v>
       </c>
       <c r="B42" s="2"/>
       <c r="C42" s="2"/>
@@ -8647,7 +8592,7 @@
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" s="2" t="s">
-        <v>540</v>
+        <v>522</v>
       </c>
       <c r="B43" s="2"/>
       <c r="C43" s="2"/>
@@ -8663,13 +8608,13 @@
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" s="54" t="s">
-        <v>537</v>
+        <v>519</v>
       </c>
       <c r="B45" s="54" t="s">
-        <v>538</v>
+        <v>520</v>
       </c>
       <c r="C45" s="54" t="s">
-        <v>544</v>
+        <v>526</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
@@ -8677,7 +8622,7 @@
         <v>1.5</v>
       </c>
       <c r="B46" s="3" t="s">
-        <v>543</v>
+        <v>525</v>
       </c>
       <c r="C46" s="2" t="str">
         <f>A46&amp;"% per "&amp;B46</f>
@@ -8686,7 +8631,7 @@
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" s="54" t="s">
-        <v>545</v>
+        <v>527</v>
       </c>
       <c r="B49" s="53"/>
       <c r="C49" s="53"/>
@@ -8695,7 +8640,7 @@
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" s="2" t="s">
-        <v>546</v>
+        <v>528</v>
       </c>
       <c r="B50" s="2"/>
       <c r="C50" s="2"/>
@@ -8704,7 +8649,7 @@
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" s="2" t="s">
-        <v>547</v>
+        <v>529</v>
       </c>
       <c r="B51" s="2"/>
       <c r="C51" s="2"/>
@@ -8713,7 +8658,7 @@
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" s="2" t="s">
-        <v>548</v>
+        <v>530</v>
       </c>
       <c r="B52" s="2"/>
       <c r="C52" s="2"/>
@@ -8722,7 +8667,7 @@
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" s="2" t="s">
-        <v>549</v>
+        <v>531</v>
       </c>
       <c r="B53" s="2"/>
       <c r="C53" s="2"/>
@@ -8731,7 +8676,7 @@
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" s="2" t="s">
-        <v>550</v>
+        <v>532</v>
       </c>
       <c r="B54" s="2"/>
       <c r="C54" s="2"/>
@@ -8740,7 +8685,7 @@
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" s="2" t="s">
-        <v>551</v>
+        <v>533</v>
       </c>
       <c r="B55" s="2"/>
       <c r="C55" s="2"/>
@@ -8749,7 +8694,7 @@
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" s="2" t="s">
-        <v>554</v>
+        <v>536</v>
       </c>
       <c r="B56" s="2"/>
       <c r="C56" s="2"/>
@@ -8758,10 +8703,10 @@
     </row>
     <row r="57" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A57" s="54" t="s">
-        <v>552</v>
+        <v>534</v>
       </c>
       <c r="B57" s="56" t="s">
-        <v>553</v>
+        <v>535</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">

</xml_diff>